<commit_message>
populating training and test data with tornado values
</commit_message>
<xml_diff>
--- a/Disaster_Locations_Coords.xlsx
+++ b/Disaster_Locations_Coords.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="8">
   <si>
     <t>Lat</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Magnitude</t>
+  </si>
+  <si>
+    <t>Length</t>
   </si>
   <si>
     <t>3</t>
@@ -392,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,8 +414,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>39.91666666666666</v>
       </c>
@@ -423,10 +429,13 @@
         <v>5.2</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>39.96666666666667</v>
       </c>
@@ -437,10 +446,13 @@
         <v>5.5</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>40.08333333333334</v>
       </c>
@@ -451,10 +463,13 @@
         <v>12.6</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>40.08333333333334</v>
       </c>
@@ -465,10 +480,13 @@
         <v>12.6</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>40.1</v>
       </c>
@@ -479,10 +497,13 @@
         <v>13.1</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>40.13333333333333</v>
       </c>
@@ -493,10 +514,13 @@
         <v>15.2</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>39.91666666666666</v>
       </c>
@@ -507,10 +531,13 @@
         <v>18.3</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>39.71666666666667</v>
       </c>
@@ -521,10 +548,13 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>39.91666666666666</v>
       </c>
@@ -535,10 +565,13 @@
         <v>21.6</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>39.65</v>
       </c>
@@ -549,10 +582,13 @@
         <v>22.7</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>39.71666666666667</v>
       </c>
@@ -563,10 +599,13 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>39.83333333333334</v>
       </c>
@@ -577,10 +616,13 @@
         <v>24.7</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>40.18333333333333</v>
       </c>
@@ -591,10 +633,13 @@
         <v>25.9</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>39.6</v>
       </c>
@@ -605,10 +650,13 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>39.58333333333334</v>
       </c>
@@ -619,10 +667,13 @@
         <v>27.1</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>40.38333333333333</v>
       </c>
@@ -633,10 +684,13 @@
         <v>29.7</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>40.01666666666667</v>
       </c>
@@ -647,10 +701,13 @@
         <v>30.4</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>39.91666666666666</v>
       </c>
@@ -661,10 +718,13 @@
         <v>30.4</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>8.699999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>40.03333333333333</v>
       </c>
@@ -675,10 +735,13 @@
         <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>40.41666666666666</v>
       </c>
@@ -689,10 +752,13 @@
         <v>31.7</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>40.16666666666666</v>
       </c>
@@ -703,10 +769,13 @@
         <v>31.9</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>40.08333333333334</v>
       </c>
@@ -717,10 +786,13 @@
         <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>40.23333333333333</v>
       </c>
@@ -731,10 +803,13 @@
         <v>35.5</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>39.48333333333333</v>
       </c>
@@ -745,10 +820,13 @@
         <v>35.8</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>40.5</v>
       </c>
@@ -759,10 +837,13 @@
         <v>36.4</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>39.78333333333333</v>
       </c>
@@ -773,10 +854,13 @@
         <v>36.8</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>40.5</v>
       </c>
@@ -787,10 +871,13 @@
         <v>37.7</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>39.75</v>
       </c>
@@ -801,10 +888,13 @@
         <v>38.2</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>40.43333333333333</v>
       </c>
@@ -815,10 +905,13 @@
         <v>38.4</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>40.35</v>
       </c>
@@ -829,10 +922,13 @@
         <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>40.5</v>
       </c>
@@ -843,10 +939,13 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>40.51666666666667</v>
       </c>
@@ -857,10 +956,13 @@
         <v>39.2</v>
       </c>
       <c r="D33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E33">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>40.38333333333333</v>
       </c>
@@ -871,10 +973,13 @@
         <v>39.6</v>
       </c>
       <c r="D34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>40.23333333333333</v>
       </c>
@@ -885,10 +990,13 @@
         <v>39.9</v>
       </c>
       <c r="D35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>39.5</v>
       </c>
@@ -899,10 +1007,13 @@
         <v>41.3</v>
       </c>
       <c r="D36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>39.48333333333333</v>
       </c>
@@ -913,10 +1024,13 @@
         <v>42.8</v>
       </c>
       <c r="D37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>40.1</v>
       </c>
@@ -927,10 +1041,13 @@
         <v>43.7</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>40.06666666666667</v>
       </c>
@@ -941,10 +1058,13 @@
         <v>45.6</v>
       </c>
       <c r="D39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E39">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>40.6</v>
       </c>
@@ -955,10 +1075,13 @@
         <v>45.6</v>
       </c>
       <c r="D40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>40.23333333333333</v>
       </c>
@@ -969,10 +1092,13 @@
         <v>46.9</v>
       </c>
       <c r="D41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>40.66666666666666</v>
       </c>
@@ -983,10 +1109,13 @@
         <v>47.3</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>40.6</v>
       </c>
@@ -997,10 +1126,13 @@
         <v>47.9</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>40.7</v>
       </c>
@@ -1011,10 +1143,13 @@
         <v>48.2</v>
       </c>
       <c r="D44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E44">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>40.66666666666666</v>
       </c>
@@ -1025,10 +1160,13 @@
         <v>48.6</v>
       </c>
       <c r="D45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E45">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>39.68333333333333</v>
       </c>
@@ -1039,10 +1177,13 @@
         <v>48.8</v>
       </c>
       <c r="D46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E46">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>40.53333333333333</v>
       </c>
@@ -1053,10 +1194,13 @@
         <v>49.7</v>
       </c>
       <c r="D47" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>39.91666666666666</v>
       </c>
@@ -1067,10 +1211,13 @@
         <v>5.2</v>
       </c>
       <c r="D48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E48">
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>40.03333333333333</v>
       </c>
@@ -1081,10 +1228,13 @@
         <v>5.5</v>
       </c>
       <c r="D49" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>40.13333333333333</v>
       </c>
@@ -1095,10 +1245,13 @@
         <v>12.6</v>
       </c>
       <c r="D50" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E50">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>40.08333333333334</v>
       </c>
@@ -1109,10 +1262,13 @@
         <v>12.6</v>
       </c>
       <c r="D51" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>40.25</v>
       </c>
@@ -1123,10 +1279,13 @@
         <v>13.1</v>
       </c>
       <c r="D52" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E52">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>40.18333333333333</v>
       </c>
@@ -1137,10 +1296,13 @@
         <v>15.2</v>
       </c>
       <c r="D53" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>39.91666666666666</v>
       </c>
@@ -1151,10 +1313,13 @@
         <v>18.3</v>
       </c>
       <c r="D54" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E54">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>39.75</v>
       </c>
@@ -1165,10 +1330,13 @@
         <v>21</v>
       </c>
       <c r="D55" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>39.91666666666666</v>
       </c>
@@ -1179,10 +1347,13 @@
         <v>21.6</v>
       </c>
       <c r="D56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E56">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>39.66666666666666</v>
       </c>
@@ -1193,10 +1364,13 @@
         <v>22.7</v>
       </c>
       <c r="D57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E57">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>39.71666666666667</v>
       </c>
@@ -1207,10 +1381,13 @@
         <v>23</v>
       </c>
       <c r="D58" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>39.93333333333333</v>
       </c>
@@ -1221,10 +1398,13 @@
         <v>24.7</v>
       </c>
       <c r="D59" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E59">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>40.26666666666667</v>
       </c>
@@ -1235,10 +1415,13 @@
         <v>25.9</v>
       </c>
       <c r="D60" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E60">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>39.61666666666667</v>
       </c>
@@ -1249,10 +1432,13 @@
         <v>26</v>
       </c>
       <c r="D61" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E61">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>39.61666666666667</v>
       </c>
@@ -1263,10 +1449,13 @@
         <v>27.1</v>
       </c>
       <c r="D62" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E62">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>40.41666666666666</v>
       </c>
@@ -1277,10 +1466,13 @@
         <v>29.7</v>
       </c>
       <c r="D63" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E63">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>39.91666666666666</v>
       </c>
@@ -1291,10 +1483,13 @@
         <v>30.4</v>
       </c>
       <c r="D64" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E64">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>39.91666666666666</v>
       </c>
@@ -1305,10 +1500,13 @@
         <v>30.4</v>
       </c>
       <c r="D65" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E65">
+        <v>8.699999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>40.1</v>
       </c>
@@ -1319,10 +1517,13 @@
         <v>31</v>
       </c>
       <c r="D66" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E66">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>40.46666666666667</v>
       </c>
@@ -1333,10 +1534,13 @@
         <v>31.7</v>
       </c>
       <c r="D67" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E67">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>40.23333333333333</v>
       </c>
@@ -1347,10 +1551,13 @@
         <v>31.9</v>
       </c>
       <c r="D68" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E68">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>40.06666666666667</v>
       </c>
@@ -1361,10 +1568,13 @@
         <v>35</v>
       </c>
       <c r="D69" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E69">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>40.16666666666666</v>
       </c>
@@ -1375,10 +1585,13 @@
         <v>35.5</v>
       </c>
       <c r="D70" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E70">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>39.7</v>
       </c>
@@ -1389,10 +1602,13 @@
         <v>35.8</v>
       </c>
       <c r="D71" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E71">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>40.5</v>
       </c>
@@ -1403,10 +1619,13 @@
         <v>36.4</v>
       </c>
       <c r="D72" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E72">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>39.91666666666666</v>
       </c>
@@ -1417,10 +1636,13 @@
         <v>36.8</v>
       </c>
       <c r="D73" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E73">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>40.55</v>
       </c>
@@ -1431,10 +1653,13 @@
         <v>37.7</v>
       </c>
       <c r="D74" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E74">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>39.75</v>
       </c>
@@ -1445,10 +1670,13 @@
         <v>38.2</v>
       </c>
       <c r="D75" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>40.6</v>
       </c>
@@ -1459,10 +1687,13 @@
         <v>38.4</v>
       </c>
       <c r="D76" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E76">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>40.35</v>
       </c>
@@ -1473,10 +1704,13 @@
         <v>39</v>
       </c>
       <c r="D77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>40.53333333333333</v>
       </c>
@@ -1487,10 +1721,13 @@
         <v>39</v>
       </c>
       <c r="D78" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>40.56666666666667</v>
       </c>
@@ -1501,10 +1738,13 @@
         <v>39.2</v>
       </c>
       <c r="D79" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E79">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>40.43333333333333</v>
       </c>
@@ -1515,10 +1755,13 @@
         <v>39.6</v>
       </c>
       <c r="D80" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E80">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>40.01666666666667</v>
       </c>
@@ -1529,10 +1772,13 @@
         <v>39.9</v>
       </c>
       <c r="D81" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E81">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>39.5</v>
       </c>
@@ -1543,10 +1789,13 @@
         <v>41.3</v>
       </c>
       <c r="D82" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E82">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>39.53333333333333</v>
       </c>
@@ -1557,10 +1806,13 @@
         <v>42.8</v>
       </c>
       <c r="D83" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E83">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>40.15</v>
       </c>
@@ -1571,10 +1823,13 @@
         <v>43.7</v>
       </c>
       <c r="D84" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E84">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>40.11666666666667</v>
       </c>
@@ -1585,10 +1840,13 @@
         <v>45.6</v>
       </c>
       <c r="D85" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E85">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>40.58333333333334</v>
       </c>
@@ -1599,10 +1857,13 @@
         <v>45.6</v>
       </c>
       <c r="D86" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>40.23333333333333</v>
       </c>
@@ -1613,10 +1874,13 @@
         <v>46.9</v>
       </c>
       <c r="D87" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>40.66666666666666</v>
       </c>
@@ -1627,10 +1891,13 @@
         <v>47.3</v>
       </c>
       <c r="D88" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>40.63333333333333</v>
       </c>
@@ -1641,10 +1908,13 @@
         <v>47.9</v>
       </c>
       <c r="D89" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90">
         <v>40.66666666666666</v>
       </c>
@@ -1655,10 +1925,13 @@
         <v>48.2</v>
       </c>
       <c r="D90" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E90">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>40.63333333333333</v>
       </c>
@@ -1669,10 +1942,13 @@
         <v>48.6</v>
       </c>
       <c r="D91" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E91">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>39.68333333333333</v>
       </c>
@@ -1683,10 +1959,13 @@
         <v>48.8</v>
       </c>
       <c r="D92" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E92">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>40.53333333333333</v>
       </c>
@@ -1697,7 +1976,10 @@
         <v>49.7</v>
       </c>
       <c r="D93" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E93">
+        <v>3.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>